<commit_message>
Mostly changes to readme. Deciding to pause the project because cannot afford what I want
</commit_message>
<xml_diff>
--- a/06_inputs/Mappings.xlsx
+++ b/06_inputs/Mappings.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Coding\R\Apartment shopping\source data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Coding\Projects\apartment_shopping\06_inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35D34B62-6F60-4F40-808A-B584F0B8E43C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FC72956-B376-40C9-830E-D9D315C924FA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{9A8069C6-F8B2-476C-84DD-BB1A0B4AE697}"/>
+    <workbookView xWindow="0" yWindow="2040" windowWidth="21600" windowHeight="11385" xr2:uid="{9A8069C6-F8B2-476C-84DD-BB1A0B4AE697}"/>
   </bookViews>
   <sheets>
     <sheet name="used_mappings" sheetId="1" r:id="rId1"/>
@@ -25,6 +25,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1226" uniqueCount="586">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1235" uniqueCount="590">
   <si>
     <t>Booli_name</t>
   </si>
@@ -1790,6 +1791,18 @@
   </si>
   <si>
     <t>virebergsolna</t>
+  </si>
+  <si>
+    <t>kåbo</t>
+  </si>
+  <si>
+    <t>fålhagen</t>
+  </si>
+  <si>
+    <t>centrum-fjärdingen</t>
+  </si>
+  <si>
+    <t>kungsängen</t>
   </si>
 </sst>
 </file>
@@ -1849,7 +1862,37 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="17">
+  <dxfs count="20">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -2027,10 +2070,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8AE61A00-CA00-4DE7-A6D0-2016F1E0A263}" name="Table1" displayName="Table1" ref="A1:B19" totalsRowShown="0">
-  <autoFilter ref="A1:B19" xr:uid="{4A9543A1-C6ED-40CC-A971-1204199618FF}"/>
-  <sortState ref="A2:B19">
-    <sortCondition ref="A1:A19"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8AE61A00-CA00-4DE7-A6D0-2016F1E0A263}" name="Table1" displayName="Table1" ref="A1:B5" totalsRowShown="0">
+  <autoFilter ref="A1:B5" xr:uid="{4A9543A1-C6ED-40CC-A971-1204199618FF}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B4">
+    <sortCondition ref="A1:A4"/>
   </sortState>
   <tableColumns count="2">
     <tableColumn id="4" xr3:uid="{BA6E9F97-2E8A-4D9D-81F3-089A7127BF02}" name="Hemnet_name"/>
@@ -2041,9 +2084,9 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F1800A77-6274-4EBD-A91A-8D8CA5AD2BBD}" name="Table13" displayName="Table13" ref="A1:F33" totalsRowShown="0">
-  <autoFilter ref="A1:F33" xr:uid="{49FF0015-CF5A-4409-BACE-DDB4A572741A}"/>
-  <sortState ref="A2:E26">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F1800A77-6274-4EBD-A91A-8D8CA5AD2BBD}" name="Table13" displayName="Table13" ref="A1:F57" totalsRowShown="0">
+  <autoFilter ref="A1:F57" xr:uid="{49FF0015-CF5A-4409-BACE-DDB4A572741A}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E26">
     <sortCondition ref="E1:E26"/>
   </sortState>
   <tableColumns count="6">
@@ -2061,12 +2104,12 @@
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{628A65A0-39F1-4D18-B921-5F19AAA12EEB}" name="Table3" displayName="Table3" ref="A1:B559" totalsRowShown="0">
   <autoFilter ref="A1:B559" xr:uid="{13B4FB00-0DDA-4C88-A612-530A33DAB3B6}"/>
-  <sortState ref="A2:B559">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B559">
     <sortCondition ref="A1:A559"/>
   </sortState>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{77B0883A-2256-4136-A5BC-CC96AB433C04}" name="scraped"/>
-    <tableColumn id="2" xr3:uid="{DF3BECA2-7713-47DE-AB27-CC94C4242B43}" name="area_mapped_to_larger_region" dataDxfId="16"/>
+    <tableColumn id="2" xr3:uid="{DF3BECA2-7713-47DE-AB27-CC94C4242B43}" name="area_mapped_to_larger_region" dataDxfId="19"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2369,16 +2412,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{867C9CE1-D522-4726-9B57-3B7551A7F9DC}">
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="33.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="33.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22.7109375" bestFit="1" customWidth="1"/>
@@ -2394,151 +2437,51 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>289</v>
+        <v>17</v>
       </c>
       <c r="B2">
-        <v>473440</v>
+        <v>925968</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>285</v>
+        <v>27</v>
       </c>
       <c r="B3">
-        <v>473339</v>
+        <v>942790</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>588</v>
       </c>
       <c r="B4">
-        <v>898740</v>
+        <v>473575</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>298</v>
+        <v>5</v>
       </c>
       <c r="B5">
-        <v>473347</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B6">
-        <v>473362</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>297</v>
-      </c>
-      <c r="B7">
-        <v>925958</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>286</v>
-      </c>
-      <c r="B8">
-        <v>473346</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>290</v>
-      </c>
-      <c r="B9">
-        <v>925972</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>293</v>
-      </c>
-      <c r="B10">
-        <v>925953</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>287</v>
-      </c>
-      <c r="B11">
-        <v>473376</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>25</v>
-      </c>
-      <c r="B12">
-        <v>898748</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>288</v>
-      </c>
-      <c r="B13">
-        <v>473385</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>291</v>
-      </c>
-      <c r="B14">
-        <v>17853</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>13</v>
-      </c>
-      <c r="B15">
-        <v>47344</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>84</v>
-      </c>
-      <c r="B16">
-        <v>898472</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>5</v>
-      </c>
-      <c r="B17">
         <v>18028</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>6</v>
-      </c>
-      <c r="B18">
-        <v>18042</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>27</v>
-      </c>
-      <c r="B19">
-        <v>942790</v>
-      </c>
-    </row>
   </sheetData>
-  <conditionalFormatting sqref="A2:A19">
-    <cfRule type="duplicateValues" dxfId="15" priority="16"/>
+  <conditionalFormatting sqref="A2">
+    <cfRule type="duplicateValues" dxfId="11" priority="9"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A3">
+    <cfRule type="duplicateValues" dxfId="10" priority="4"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A4">
+    <cfRule type="duplicateValues" dxfId="9" priority="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A5">
+    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A5">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -2549,10 +2492,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D37F582-6F4E-4CA8-BCEC-157E963C8490}">
-  <dimension ref="A1:F33"/>
+  <dimension ref="A1:F57"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C55" sqref="C55:D55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3077,21 +3020,202 @@
       </c>
       <c r="F33" s="1"/>
     </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C34" t="s">
+        <v>586</v>
+      </c>
+      <c r="D34">
+        <v>473560</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C36" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C37" t="s">
+        <v>588</v>
+      </c>
+      <c r="D37">
+        <v>473575</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C38" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C39" t="s">
+        <v>17</v>
+      </c>
+      <c r="D39">
+        <v>925968</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C40" t="s">
+        <v>289</v>
+      </c>
+      <c r="D40">
+        <v>473440</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C41" t="s">
+        <v>285</v>
+      </c>
+      <c r="D41">
+        <v>473339</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C42" t="s">
+        <v>18</v>
+      </c>
+      <c r="D42">
+        <v>898740</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C43" t="s">
+        <v>298</v>
+      </c>
+      <c r="D43">
+        <v>473347</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C44" t="s">
+        <v>21</v>
+      </c>
+      <c r="D44">
+        <v>473362</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C45" t="s">
+        <v>297</v>
+      </c>
+      <c r="D45">
+        <v>925958</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C46" t="s">
+        <v>286</v>
+      </c>
+      <c r="D46">
+        <v>473346</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C47" t="s">
+        <v>290</v>
+      </c>
+      <c r="D47">
+        <v>925972</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C48" t="s">
+        <v>293</v>
+      </c>
+      <c r="D48">
+        <v>925953</v>
+      </c>
+    </row>
+    <row r="49" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C49" t="s">
+        <v>287</v>
+      </c>
+      <c r="D49">
+        <v>473376</v>
+      </c>
+    </row>
+    <row r="50" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C50" t="s">
+        <v>25</v>
+      </c>
+      <c r="D50">
+        <v>898748</v>
+      </c>
+    </row>
+    <row r="51" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C51" t="s">
+        <v>288</v>
+      </c>
+      <c r="D51">
+        <v>473385</v>
+      </c>
+    </row>
+    <row r="52" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C52" t="s">
+        <v>291</v>
+      </c>
+      <c r="D52">
+        <v>17853</v>
+      </c>
+    </row>
+    <row r="53" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C53" t="s">
+        <v>13</v>
+      </c>
+      <c r="D53">
+        <v>47344</v>
+      </c>
+    </row>
+    <row r="54" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C54" t="s">
+        <v>84</v>
+      </c>
+      <c r="D54">
+        <v>898472</v>
+      </c>
+    </row>
+    <row r="55" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C55" t="s">
+        <v>5</v>
+      </c>
+      <c r="D55">
+        <v>18028</v>
+      </c>
+    </row>
+    <row r="56" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C56" t="s">
+        <v>6</v>
+      </c>
+      <c r="D56">
+        <v>18042</v>
+      </c>
+    </row>
+    <row r="57" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C57" t="s">
+        <v>27</v>
+      </c>
+      <c r="D57">
+        <v>942790</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="A2:A6 A8:A33">
-    <cfRule type="duplicateValues" dxfId="14" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="8" priority="6"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C2:C33">
-    <cfRule type="duplicateValues" dxfId="13" priority="4"/>
+  <conditionalFormatting sqref="C2:C57">
+    <cfRule type="duplicateValues" dxfId="7" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E6 E8:E33">
-    <cfRule type="duplicateValues" dxfId="12" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A7">
-    <cfRule type="duplicateValues" dxfId="11" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E7">
-    <cfRule type="duplicateValues" dxfId="10" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C40:C57">
+    <cfRule type="duplicateValues" dxfId="3" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -3104,7 +3228,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FF99511-1B23-480D-B47D-D53711434B9A}">
   <dimension ref="A1:B559"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -7589,7 +7713,7 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="A2:A559">
-    <cfRule type="duplicateValues" dxfId="5" priority="193"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="193"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>